<commit_message>
Srikanth P | Name Pro Angular | Initial Commit
</commit_message>
<xml_diff>
--- a/documents/3_Artifacts_Name_Pro_By_Team_ORION.xlsx
+++ b/documents/3_Artifacts_Name_Pro_By_Team_ORION.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dev Krishna Mishra\Desktop\Hackathon\Artifacts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A3163451-7D90-4048-8014-6602AAF0832A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6880227-AB86-4F32-83CF-600549F79088}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="522" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="522" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Agile Team" sheetId="22" r:id="rId1"/>
@@ -40,20 +40,20 @@
     <definedName name="PBTrend">OFFSET(#REF!,1,0,#REF!,1)</definedName>
     <definedName name="PlannedSpeed">OFFSET(#REF!,1,0,#REF!,1)</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'Product Backlog'!$A:$J</definedName>
-    <definedName name="ProductBacklog">'Product Backlog'!$A$9:$J$187</definedName>
+    <definedName name="ProductBacklog">'Product Backlog'!$A$9:$J$185</definedName>
     <definedName name="RealizedSpeed">OFFSET(#REF!,1,0,#REF!,1)</definedName>
     <definedName name="RealValues" localSheetId="2">OFFSET('Sprint 1'!$G$5,0,0,1,'Sprint 1'!DoneDays)</definedName>
     <definedName name="RealValues" localSheetId="3">OFFSET('Sprint 2'!$G$5,0,0,1,'Sprint 2'!DoneDays)</definedName>
     <definedName name="RealValues" localSheetId="4">OFFSET('Sprint 3'!$G$5,0,0,1,'Sprint 3'!DoneDays)</definedName>
-    <definedName name="Sprint">'Product Backlog'!$H$10:$H$187</definedName>
+    <definedName name="Sprint">'Product Backlog'!$H$10:$H$185</definedName>
     <definedName name="SprintCount">#REF!</definedName>
     <definedName name="SprintsInTrend">#REF!</definedName>
     <definedName name="SprintTasks" localSheetId="2">'Sprint 1'!$A$9:$AE$58</definedName>
     <definedName name="SprintTasks" localSheetId="3">'Sprint 2'!$A$9:$AE$58</definedName>
     <definedName name="SprintTasks" localSheetId="4">'Sprint 3'!$A$9:$AE$58</definedName>
     <definedName name="SprintTasks">#REF!</definedName>
-    <definedName name="Status">'Product Backlog'!$F$10:$F$187</definedName>
-    <definedName name="StoryName">'Product Backlog'!$D$10:$D$187</definedName>
+    <definedName name="Status">'Product Backlog'!$F$10:$F$185</definedName>
+    <definedName name="StoryName">'Product Backlog'!$D$10:$D$185</definedName>
     <definedName name="TaskRows" localSheetId="2">'Sprint 1'!$B$6</definedName>
     <definedName name="TaskRows" localSheetId="3">'Sprint 2'!$B$6</definedName>
     <definedName name="TaskRows" localSheetId="4">'Sprint 3'!$B$6</definedName>
@@ -256,7 +256,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="123">
   <si>
     <t>Status</t>
   </si>
@@ -276,9 +276,6 @@
     <t>Totals</t>
   </si>
   <si>
-    <t>Planned</t>
-  </si>
-  <si>
     <t>Story ID</t>
   </si>
   <si>
@@ -390,16 +387,10 @@
     <t>Product Backlog (Stories)</t>
   </si>
   <si>
-    <t>Integration with portals and collaboration tools</t>
-  </si>
-  <si>
     <t>Standard Pronunciation</t>
   </si>
   <si>
     <t>Capability to manage the standard pronunciation of Employee names based on user roles along with the ability to search and play the existing audio samples for other employees</t>
-  </si>
-  <si>
-    <t>Integration of the name pronunciation feature with internal portals and other collaboration tools</t>
   </si>
   <si>
     <t>Login - UI Display</t>
@@ -413,15 +404,6 @@
 Then I should be able to login to the platform</t>
   </si>
   <si>
-    <t xml:space="preserve"> Login - SSO implementation</t>
-  </si>
-  <si>
-    <t>Integration and Collaboration</t>
-  </si>
-  <si>
-    <t>NA</t>
-  </si>
-  <si>
     <t>Dashboard - UI Display</t>
   </si>
   <si>
@@ -431,16 +413,10 @@
     <t>Admin - UI Display</t>
   </si>
   <si>
-    <t>Implement SSO so that employees can login using their existing AD-ENT credentials</t>
-  </si>
-  <si>
     <t>Allow users to search for other employees by entering their details</t>
   </si>
   <si>
     <t>Allow playback of standard pronunciation for users</t>
-  </si>
-  <si>
-    <t>Allow integration of APIs to internal portals like Teamworks, Workday and Outlook</t>
   </si>
   <si>
     <t>Given I am the product owner of a different product
@@ -448,11 +424,6 @@
 Then I should be able to integrate in internal portals</t>
   </si>
   <si>
-    <t>Given I am a Wells Fargo employee
-When I enter my AD-ENT credentials
-Then I should be routed to the interface</t>
-  </si>
-  <si>
     <t>Given I have logged in to the interface
 When I search for a user
 Then I should be able to look up the user profile</t>
@@ -473,9 +444,6 @@
 Approve/Reject requests - Administrator</t>
   </si>
   <si>
-    <t>Smooth integration with internal portals and/or collaboration tools such as Outlook, Teams, Workday</t>
-  </si>
-  <si>
     <t>Given I am a Wells Fargo employee
 When I have logged in to the platform as an Employee
 Then I should be routed to the Dashboard</t>
@@ -682,21 +650,31 @@
     <t>My Profile - Logout</t>
   </si>
   <si>
-    <t>Documentation - Playbook</t>
-  </si>
-  <si>
-    <t>Documentation - Technology Stack</t>
-  </si>
-  <si>
     <t>Details of the technology stack for the application</t>
-  </si>
-  <si>
-    <t>Detailed documentation of the steps to be performed for the available features on the application</t>
   </si>
   <si>
     <t>Given the application UI and API have been developed
 When I click on the 'Download Playbook' link
 Then I should be able to download the application playbook</t>
+  </si>
+  <si>
+    <t>Stepwise documentation of the actions to be performed on the application</t>
+  </si>
+  <si>
+    <t>Artifacts and Deliverables</t>
+  </si>
+  <si>
+    <t>Documentation of artifacts and deliverables to support the application purpose and funtionality</t>
+  </si>
+  <si>
+    <t>Application Playbook
+Technology Stack</t>
+  </si>
+  <si>
+    <t>Application Playbook</t>
+  </si>
+  <si>
+    <t>Technology Stack</t>
   </si>
 </sst>
 </file>
@@ -1033,29 +1011,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="101">
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor indexed="10"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="43"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="42"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="107">
     <dxf>
       <fill>
         <patternFill>
@@ -1772,6 +1728,72 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor indexed="10"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="43"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="42"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor indexed="10"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="43"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="42"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor indexed="10"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="43"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="42"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -3927,7 +3949,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
@@ -3944,63 +3966,63 @@
   <sheetData>
     <row r="1" spans="1:2" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="29" t="s">
         <v>22</v>
-      </c>
-      <c r="B4" s="29" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A5" s="30" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B5" s="30" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A6" s="30" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B6" s="30" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A7" s="30" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B7" s="30" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A8" s="30" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B8" s="30" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A9" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="30" t="s">
         <v>26</v>
-      </c>
-      <c r="B9" s="30" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A10" s="31" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B10" s="31" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="18" x14ac:dyDescent="0.35">
@@ -4021,10 +4043,10 @@
   <sheetPr codeName="Sheet2">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:M77"/>
+  <dimension ref="A1:M75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -4044,23 +4066,23 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B1" s="1"/>
     </row>
     <row r="3" spans="1:10" s="8" customFormat="1" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="19" t="s">
         <v>35</v>
-      </c>
-      <c r="B3" s="19" t="s">
-        <v>36</v>
       </c>
       <c r="C3" s="19"/>
       <c r="D3" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>37</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>38</v>
       </c>
       <c r="F3" s="17"/>
       <c r="G3" s="17"/>
@@ -4073,14 +4095,14 @@
         <v>1</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C4" s="21"/>
       <c r="D4" s="22" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E4" s="22" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="F4" s="15"/>
       <c r="G4" s="15"/>
@@ -4091,14 +4113,14 @@
         <v>2</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="C5" s="23"/>
       <c r="D5" s="22" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="E5" s="25" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="F5" s="15"/>
       <c r="G5" s="15"/>
@@ -4109,14 +4131,14 @@
         <v>3</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>52</v>
+        <v>118</v>
       </c>
       <c r="C6" s="23"/>
       <c r="D6" s="22" t="s">
-        <v>47</v>
+        <v>119</v>
       </c>
       <c r="E6" s="25" t="s">
-        <v>68</v>
+        <v>120</v>
       </c>
       <c r="F6" s="15"/>
       <c r="G6" s="15"/>
@@ -4132,14 +4154,14 @@
     </row>
     <row r="8" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="28" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B8" s="28"/>
       <c r="C8" s="26"/>
       <c r="D8" s="22"/>
       <c r="E8" s="22"/>
       <c r="F8" s="27" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G8" s="16"/>
       <c r="H8" s="16"/>
@@ -4148,34 +4170,34 @@
     </row>
     <row r="9" spans="1:10" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="24" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9" s="24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C9" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="D9" s="24" t="s">
+      <c r="E9" s="24" t="s">
         <v>37</v>
-      </c>
-      <c r="E9" s="24" t="s">
-        <v>38</v>
       </c>
       <c r="F9" s="18" t="s">
         <v>0</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H9" s="18" t="s">
         <v>4</v>
       </c>
       <c r="I9" s="24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J9" s="24" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -4183,19 +4205,19 @@
         <v>1</v>
       </c>
       <c r="B10" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="C10" s="22" t="s">
-        <v>48</v>
-      </c>
       <c r="D10" s="22" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E10" s="22" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F10" s="16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G10" s="16">
         <v>3</v>
@@ -4211,19 +4233,19 @@
         <v>2</v>
       </c>
       <c r="B11" s="22" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C11" s="22" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="D11" s="22" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="E11" s="22" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="F11" s="16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G11" s="16">
         <v>5</v>
@@ -4239,19 +4261,19 @@
         <v>3</v>
       </c>
       <c r="B12" s="22" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C12" s="22" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="D12" s="22" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="E12" s="22" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="F12" s="16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G12" s="16">
         <v>3</v>
@@ -4267,19 +4289,19 @@
         <v>4</v>
       </c>
       <c r="B13" s="22" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C13" s="22" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="D13" s="22" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="E13" s="22" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="F13" s="16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G13" s="16">
         <v>2</v>
@@ -4295,19 +4317,19 @@
         <v>5</v>
       </c>
       <c r="B14" s="22" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C14" s="22" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="D14" s="22" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="E14" s="22" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="F14" s="16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G14" s="16">
         <v>3</v>
@@ -4323,19 +4345,19 @@
         <v>6</v>
       </c>
       <c r="B15" s="22" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C15" s="22" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="D15" s="22" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="E15" s="22" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="F15" s="16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G15" s="16">
         <v>2</v>
@@ -4351,19 +4373,19 @@
         <v>7</v>
       </c>
       <c r="B16" s="22" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C16" s="22" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="D16" s="22" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="E16" s="22" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="F16" s="16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G16" s="16">
         <v>3</v>
@@ -4379,19 +4401,19 @@
         <v>8</v>
       </c>
       <c r="B17" s="22" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="C17" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="D17" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="E17" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="D17" s="22" t="s">
-        <v>81</v>
-      </c>
-      <c r="E17" s="22" t="s">
-        <v>90</v>
-      </c>
       <c r="F17" s="16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G17" s="16">
         <v>2</v>
@@ -4407,19 +4429,19 @@
         <v>9</v>
       </c>
       <c r="B18" s="22" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="C18" s="22" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="D18" s="22" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="E18" s="22" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="F18" s="16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G18" s="16">
         <v>3</v>
@@ -4435,19 +4457,19 @@
         <v>10</v>
       </c>
       <c r="B19" s="22" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="C19" s="22" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="D19" s="22" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="E19" s="22" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="F19" s="16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G19" s="16">
         <v>3</v>
@@ -4463,19 +4485,19 @@
         <v>11</v>
       </c>
       <c r="B20" s="22" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="C20" s="22" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="D20" s="22" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="E20" s="22" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="F20" s="16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G20" s="16">
         <v>2</v>
@@ -4491,19 +4513,19 @@
         <v>12</v>
       </c>
       <c r="B21" s="22" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="C21" s="22" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="D21" s="22" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="E21" s="22" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="F21" s="16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G21" s="16">
         <v>2</v>
@@ -4519,19 +4541,19 @@
         <v>13</v>
       </c>
       <c r="B22" s="22" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C22" s="22" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="D22" s="22" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="E22" s="22" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="F22" s="16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G22" s="16">
         <v>1</v>
@@ -4547,19 +4569,19 @@
         <v>14</v>
       </c>
       <c r="B23" s="22" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="C23" s="22" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="D23" s="22" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="E23" s="22" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="F23" s="16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G23" s="16">
         <v>3</v>
@@ -4575,19 +4597,19 @@
         <v>15</v>
       </c>
       <c r="B24" s="22" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="C24" s="22" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="D24" s="22" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="E24" s="22" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="F24" s="16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G24" s="16">
         <v>3</v>
@@ -4603,19 +4625,19 @@
         <v>16</v>
       </c>
       <c r="B25" s="22" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="C25" s="22" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="D25" s="22" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="E25" s="22" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="F25" s="16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G25" s="16">
         <v>2</v>
@@ -4631,19 +4653,19 @@
         <v>17</v>
       </c>
       <c r="B26" s="22" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="C26" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="D26" s="22" t="s">
         <v>96</v>
       </c>
-      <c r="D26" s="22" t="s">
-        <v>106</v>
-      </c>
       <c r="E26" s="22" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="F26" s="16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G26" s="16">
         <v>2</v>
@@ -4659,19 +4681,19 @@
         <v>18</v>
       </c>
       <c r="B27" s="22" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="C27" s="22" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="D27" s="22" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="E27" s="22" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="F27" s="16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G27" s="16">
         <v>2</v>
@@ -4687,19 +4709,19 @@
         <v>19</v>
       </c>
       <c r="B28" s="22" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="C28" s="22" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="D28" s="22" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="E28" s="22" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="F28" s="16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G28" s="16">
         <v>3</v>
@@ -4715,19 +4737,19 @@
         <v>20</v>
       </c>
       <c r="B29" s="22" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="C29" s="22" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="D29" s="22" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="E29" s="22" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="F29" s="16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G29" s="16">
         <v>3</v>
@@ -4743,19 +4765,19 @@
         <v>21</v>
       </c>
       <c r="B30" s="22" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="C30" s="22" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="D30" s="22" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="E30" s="22" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="F30" s="16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G30" s="16">
         <v>3</v>
@@ -4771,19 +4793,19 @@
         <v>22</v>
       </c>
       <c r="B31" s="22" t="s">
-        <v>52</v>
+        <v>118</v>
       </c>
       <c r="C31" s="22" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="D31" s="22" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
       <c r="E31" s="22" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="F31" s="16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G31" s="16">
         <v>5</v>
@@ -4799,19 +4821,19 @@
         <v>23</v>
       </c>
       <c r="B32" s="22" t="s">
-        <v>52</v>
+        <v>118</v>
       </c>
       <c r="C32" s="22" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="D32" s="22" t="s">
-        <v>127</v>
+        <v>115</v>
       </c>
       <c r="E32" s="22" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="F32" s="16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G32" s="16">
         <v>5</v>
@@ -4822,83 +4844,27 @@
       <c r="I32" s="22"/>
       <c r="J32" s="22"/>
     </row>
-    <row r="33" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="22">
-        <v>24</v>
-      </c>
-      <c r="B33" s="22" t="s">
-        <v>52</v>
-      </c>
-      <c r="C33" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="D33" s="22" t="s">
-        <v>60</v>
-      </c>
-      <c r="E33" s="22" t="s">
-        <v>61</v>
-      </c>
-      <c r="F33" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="G33" s="16">
-        <v>5</v>
-      </c>
-      <c r="H33" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="I33" s="22"/>
-      <c r="J33" s="22"/>
-    </row>
-    <row r="34" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="22">
-        <v>25</v>
-      </c>
-      <c r="B34" s="22" t="s">
-        <v>52</v>
-      </c>
-      <c r="C34" s="22" t="s">
-        <v>51</v>
-      </c>
-      <c r="D34" s="22" t="s">
-        <v>57</v>
-      </c>
-      <c r="E34" s="22" t="s">
-        <v>62</v>
-      </c>
-      <c r="F34" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="G34" s="16">
-        <v>3</v>
-      </c>
-      <c r="H34" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="I34" s="22"/>
-      <c r="J34" s="22"/>
-    </row>
-    <row r="35" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="53" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D53" s="4"/>
-      <c r="E53" s="4"/>
-    </row>
-    <row r="61" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="M61" s="6"/>
-    </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="J66" s="7"/>
-    </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A77" s="4"/>
-      <c r="B77" s="4"/>
-      <c r="C77" s="4"/>
-      <c r="D77" s="4"/>
-      <c r="E77" s="4"/>
-      <c r="I77" s="4"/>
+    <row r="33" ht="26.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="51" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D51" s="4"/>
+      <c r="E51" s="4"/>
+    </row>
+    <row r="59" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="M59" s="6"/>
+    </row>
+    <row r="64" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="J64" s="7"/>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A75" s="4"/>
+      <c r="B75" s="4"/>
+      <c r="C75" s="4"/>
+      <c r="D75" s="4"/>
+      <c r="E75" s="4"/>
+      <c r="I75" s="4"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:K64">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:K62">
     <sortCondition ref="H5"/>
     <sortCondition ref="F5"/>
   </sortState>
@@ -4910,209 +4876,220 @@
     <mergeCell ref="A8:B8"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="J68:J76 F69:F70 A35:C76 J47:J65 D35:I68 A78:J187 D71:I76 J35:J45 A9:C9 F9:J9 D3:J3 A3:B3 C17:J17 A17 A10:A14 C10:J14 A26:J27 A29:J30 A33:J34">
-    <cfRule type="expression" dxfId="100" priority="85" stopIfTrue="1">
+  <conditionalFormatting sqref="J66:J74 F67:F68 A33:C74 J45:J63 D33:I66 A76:J185 D69:I74 J33:J43 A9:C9 F9:J9 D3:J3 A3:B3 C17:J17 A17 A10:A14 C10:J14 A26:J27 A29:J30">
+    <cfRule type="expression" dxfId="106" priority="91" stopIfTrue="1">
       <formula>$F3="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="99" priority="86" stopIfTrue="1">
+    <cfRule type="expression" dxfId="105" priority="92" stopIfTrue="1">
       <formula>$F3="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="98" priority="87" stopIfTrue="1">
+    <cfRule type="expression" dxfId="104" priority="93" stopIfTrue="1">
       <formula>$F3="Removed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J77">
-    <cfRule type="expression" dxfId="97" priority="88" stopIfTrue="1">
-      <formula>$F67="Done"</formula>
+  <conditionalFormatting sqref="J75">
+    <cfRule type="expression" dxfId="103" priority="94" stopIfTrue="1">
+      <formula>$F65="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="96" priority="89" stopIfTrue="1">
-      <formula>$F67="Ongoing"</formula>
+    <cfRule type="expression" dxfId="102" priority="95" stopIfTrue="1">
+      <formula>$F65="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="95" priority="90" stopIfTrue="1">
-      <formula>$F67="Removed"</formula>
+    <cfRule type="expression" dxfId="101" priority="96" stopIfTrue="1">
+      <formula>$F65="Removed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J66:J67">
-    <cfRule type="expression" dxfId="94" priority="91" stopIfTrue="1">
+  <conditionalFormatting sqref="J64:J65">
+    <cfRule type="expression" dxfId="100" priority="97" stopIfTrue="1">
       <formula>#REF!="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="93" priority="92" stopIfTrue="1">
+    <cfRule type="expression" dxfId="99" priority="98" stopIfTrue="1">
       <formula>#REF!="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="92" priority="93" stopIfTrue="1">
+    <cfRule type="expression" dxfId="98" priority="99" stopIfTrue="1">
       <formula>#REF!="Removed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J46">
-    <cfRule type="expression" dxfId="91" priority="94" stopIfTrue="1">
+  <conditionalFormatting sqref="J44">
+    <cfRule type="expression" dxfId="97" priority="100" stopIfTrue="1">
       <formula>#REF!="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="90" priority="95" stopIfTrue="1">
+    <cfRule type="expression" dxfId="96" priority="101" stopIfTrue="1">
       <formula>#REF!="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="89" priority="96" stopIfTrue="1">
+    <cfRule type="expression" dxfId="95" priority="102" stopIfTrue="1">
       <formula>#REF!="Removed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9">
-    <cfRule type="expression" dxfId="88" priority="46" stopIfTrue="1">
+    <cfRule type="expression" dxfId="94" priority="52" stopIfTrue="1">
       <formula>$F9="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="87" priority="47" stopIfTrue="1">
+    <cfRule type="expression" dxfId="93" priority="53" stopIfTrue="1">
       <formula>$F9="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="86" priority="48" stopIfTrue="1">
+    <cfRule type="expression" dxfId="92" priority="54" stopIfTrue="1">
       <formula>$F9="Removed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9">
-    <cfRule type="expression" dxfId="85" priority="43" stopIfTrue="1">
+    <cfRule type="expression" dxfId="91" priority="49" stopIfTrue="1">
       <formula>$F9="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="84" priority="44" stopIfTrue="1">
+    <cfRule type="expression" dxfId="90" priority="50" stopIfTrue="1">
       <formula>$F9="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="83" priority="45" stopIfTrue="1">
+    <cfRule type="expression" dxfId="89" priority="51" stopIfTrue="1">
       <formula>$F9="Removed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A15:A16 C15:J16">
-    <cfRule type="expression" dxfId="82" priority="37" stopIfTrue="1">
+    <cfRule type="expression" dxfId="88" priority="43" stopIfTrue="1">
       <formula>$F15="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="81" priority="38" stopIfTrue="1">
+    <cfRule type="expression" dxfId="87" priority="44" stopIfTrue="1">
       <formula>$F15="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="80" priority="39" stopIfTrue="1">
+    <cfRule type="expression" dxfId="86" priority="45" stopIfTrue="1">
       <formula>$F15="Removed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C18:J18 A18">
-    <cfRule type="expression" dxfId="79" priority="34" stopIfTrue="1">
+    <cfRule type="expression" dxfId="85" priority="40" stopIfTrue="1">
       <formula>$F18="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="78" priority="35" stopIfTrue="1">
+    <cfRule type="expression" dxfId="84" priority="41" stopIfTrue="1">
       <formula>$F18="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="77" priority="36" stopIfTrue="1">
+    <cfRule type="expression" dxfId="83" priority="42" stopIfTrue="1">
       <formula>$F18="Removed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20:J20 A20">
-    <cfRule type="expression" dxfId="76" priority="31" stopIfTrue="1">
+    <cfRule type="expression" dxfId="82" priority="37" stopIfTrue="1">
       <formula>$F20="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="75" priority="32" stopIfTrue="1">
+    <cfRule type="expression" dxfId="81" priority="38" stopIfTrue="1">
       <formula>$F20="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="74" priority="33" stopIfTrue="1">
+    <cfRule type="expression" dxfId="80" priority="39" stopIfTrue="1">
       <formula>$F20="Removed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19:J19 A19">
-    <cfRule type="expression" dxfId="73" priority="28" stopIfTrue="1">
+    <cfRule type="expression" dxfId="79" priority="34" stopIfTrue="1">
       <formula>$F19="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="72" priority="29" stopIfTrue="1">
+    <cfRule type="expression" dxfId="78" priority="35" stopIfTrue="1">
       <formula>$F19="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="71" priority="30" stopIfTrue="1">
+    <cfRule type="expression" dxfId="77" priority="36" stopIfTrue="1">
       <formula>$F19="Removed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C21:J21 A21">
-    <cfRule type="expression" dxfId="70" priority="25" stopIfTrue="1">
+    <cfRule type="expression" dxfId="76" priority="31" stopIfTrue="1">
       <formula>$F21="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="69" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="75" priority="32" stopIfTrue="1">
       <formula>$F21="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="68" priority="27" stopIfTrue="1">
+    <cfRule type="expression" dxfId="74" priority="33" stopIfTrue="1">
       <formula>$F21="Removed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A23:J23">
-    <cfRule type="expression" dxfId="67" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="73" priority="28" stopIfTrue="1">
       <formula>$F23="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="66" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="72" priority="29" stopIfTrue="1">
       <formula>$F23="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="65" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="71" priority="30" stopIfTrue="1">
       <formula>$F23="Removed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A25:J25">
-    <cfRule type="expression" dxfId="64" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="70" priority="25" stopIfTrue="1">
       <formula>$F25="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="63" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="69" priority="26" stopIfTrue="1">
       <formula>$F25="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="62" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="68" priority="27" stopIfTrue="1">
       <formula>$F25="Removed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A24:J24">
-    <cfRule type="expression" dxfId="61" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="67" priority="22" stopIfTrue="1">
       <formula>$F24="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="60" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="66" priority="23" stopIfTrue="1">
       <formula>$F24="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="59" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="65" priority="24" stopIfTrue="1">
       <formula>$F24="Removed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A28:J28">
-    <cfRule type="expression" dxfId="58" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="64" priority="16" stopIfTrue="1">
       <formula>$F28="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="57" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="63" priority="17" stopIfTrue="1">
       <formula>$F28="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="56" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="62" priority="18" stopIfTrue="1">
       <formula>$F28="Removed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A22:J22">
-    <cfRule type="expression" dxfId="55" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="61" priority="13" stopIfTrue="1">
       <formula>$F22="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="54" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="60" priority="14" stopIfTrue="1">
       <formula>$F22="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="53" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="59" priority="15" stopIfTrue="1">
       <formula>$F22="Removed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A31:J31">
-    <cfRule type="expression" dxfId="52" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="58" priority="10" stopIfTrue="1">
       <formula>$F31="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="51" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="57" priority="11" stopIfTrue="1">
       <formula>$F31="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="50" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="56" priority="12" stopIfTrue="1">
       <formula>$F31="Removed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A32:J32">
-    <cfRule type="expression" dxfId="2" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="49" priority="7" stopIfTrue="1">
       <formula>$F32="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="48" priority="8" stopIfTrue="1">
       <formula>$F32="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="47" priority="9" stopIfTrue="1">
       <formula>$F32="Removed"</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="B10:B21">
+    <cfRule type="expression" dxfId="46" priority="4" stopIfTrue="1">
+      <formula>$F10="Done"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="45" priority="5" stopIfTrue="1">
+      <formula>$F10="Ongoing"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="44" priority="6" stopIfTrue="1">
+      <formula>$F10="Removed"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="F78:F187 F9 F28:F76" xr:uid="{00000000-0002-0000-0200-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="F76:F185 F9 F28:F74" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>"Planned,Ongoing,Done,Removed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F34 F10:F27" xr:uid="{00000000-0002-0000-0200-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F10:F27" xr:uid="{00000000-0002-0000-0200-000001000000}">
       <formula1>"Planned,Ongoing,Done,Removed"</formula1>
     </dataValidation>
   </dataValidations>
@@ -5208,7 +5185,7 @@
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" s="32" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="B4" s="33">
         <v>4</v>
@@ -5220,7 +5197,7 @@
         <v>2</v>
       </c>
       <c r="G4" s="35" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="H4" s="35"/>
       <c r="I4" s="35"/>
@@ -5249,7 +5226,7 @@
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" s="32" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B5" s="33">
         <v>2</v>
@@ -5366,7 +5343,7 @@
     </row>
     <row r="6" spans="1:31" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" s="37" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6" s="38">
         <f>IF(COUNTA(A10:A237)=0,1,COUNTA(A10:A237))</f>
@@ -5374,7 +5351,7 @@
       </c>
       <c r="C6" s="38"/>
       <c r="D6" s="37" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E6" s="38">
         <f ca="1">IF(COUNTIF(G5:AE5,"&gt;0")=0,1,COUNTIF(G5:AE5,"&gt;0"))</f>
@@ -5484,12 +5461,12 @@
     </row>
     <row r="7" spans="1:31" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" s="39" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B7" s="37"/>
       <c r="C7" s="37"/>
       <c r="D7" s="37" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E7" s="38"/>
       <c r="F7" s="38"/>
@@ -5596,12 +5573,12 @@
     </row>
     <row r="8" spans="1:31" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" s="39" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B8" s="37"/>
       <c r="C8" s="37"/>
       <c r="D8" s="37" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E8" s="38">
         <f ca="1">IF(DoneDays&gt;B5,B5,DoneDays)</f>
@@ -5687,13 +5664,13 @@
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" s="32" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B9" s="40" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C9" s="40" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D9" s="40" t="s">
         <v>1</v>
@@ -5806,7 +5783,7 @@
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B10" s="10">
         <v>1</v>
@@ -5815,10 +5792,10 @@
         <v>3</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F10" s="10">
         <v>3</v>
@@ -5836,7 +5813,7 @@
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B11" s="10">
         <v>2</v>
@@ -5845,10 +5822,10 @@
         <v>5</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F11" s="10">
         <v>5</v>
@@ -5868,7 +5845,7 @@
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B12" s="10">
         <v>3</v>
@@ -5877,10 +5854,10 @@
         <v>3</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F12" s="10">
         <v>3</v>
@@ -5900,7 +5877,7 @@
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="B13" s="10">
         <v>4</v>
@@ -5909,10 +5886,10 @@
         <v>2</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F13" s="10">
         <v>2</v>
@@ -5938,7 +5915,7 @@
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="B14" s="3">
         <v>5</v>
@@ -5947,10 +5924,10 @@
         <v>3</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F14" s="3">
         <v>3</v>
@@ -5978,7 +5955,7 @@
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="B15" s="3">
         <v>6</v>
@@ -5987,10 +5964,10 @@
         <v>2</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F15" s="3">
         <v>2</v>
@@ -6012,7 +5989,7 @@
     </row>
     <row r="16" spans="1:31" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="B16" s="3">
         <v>7</v>
@@ -6021,10 +5998,10 @@
         <v>3</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F16" s="3">
         <v>3</v>
@@ -6944,32 +6921,32 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A10:AE53">
-    <cfRule type="expression" dxfId="43" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="40" priority="7" stopIfTrue="1">
       <formula>$E10="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="42" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="39" priority="8" stopIfTrue="1">
       <formula>$E10="Ongoing"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10:C14">
-    <cfRule type="expression" dxfId="41" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="38" priority="4" stopIfTrue="1">
       <formula>$G10="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="40" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="37" priority="5" stopIfTrue="1">
       <formula>$G10="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="39" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="36" priority="6" stopIfTrue="1">
       <formula>$G10="Removed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15:C16">
-    <cfRule type="expression" dxfId="38" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="35" priority="1" stopIfTrue="1">
       <formula>$G15="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="37" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="34" priority="2" stopIfTrue="1">
       <formula>$G15="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="36" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="33" priority="3" stopIfTrue="1">
       <formula>$G15="Removed"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7070,7 +7047,7 @@
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" s="32" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="B4" s="33">
         <v>4</v>
@@ -7082,7 +7059,7 @@
         <v>2</v>
       </c>
       <c r="G4" s="41" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="H4" s="45"/>
       <c r="I4" s="45"/>
@@ -7111,7 +7088,7 @@
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" s="32" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B5" s="33">
         <v>2</v>
@@ -7228,7 +7205,7 @@
     </row>
     <row r="6" spans="1:31" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" s="37" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6" s="38">
         <f>IF(COUNTA(A10:A237)=0,1,COUNTA(A10:A237))</f>
@@ -7236,7 +7213,7 @@
       </c>
       <c r="C6" s="38"/>
       <c r="D6" s="37" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E6" s="38">
         <f ca="1">IF(COUNTIF(G5:AE5,"&gt;0")=0,1,COUNTIF(G5:AE5,"&gt;0"))</f>
@@ -7346,12 +7323,12 @@
     </row>
     <row r="7" spans="1:31" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" s="39" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B7" s="37"/>
       <c r="C7" s="37"/>
       <c r="D7" s="37" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E7" s="38"/>
       <c r="F7" s="38"/>
@@ -7458,12 +7435,12 @@
     </row>
     <row r="8" spans="1:31" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" s="39" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B8" s="37"/>
       <c r="C8" s="37"/>
       <c r="D8" s="37" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E8" s="38">
         <f ca="1">IF(DoneDays&gt;B5,B5,DoneDays)</f>
@@ -7549,13 +7526,13 @@
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" s="32" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B9" s="40" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C9" s="40" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D9" s="40" t="s">
         <v>1</v>
@@ -7668,7 +7645,7 @@
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="B10" s="10">
         <v>8</v>
@@ -7677,10 +7654,10 @@
         <v>2</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F10" s="10">
         <v>2</v>
@@ -7696,7 +7673,7 @@
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="B11" s="10">
         <v>9</v>
@@ -7705,10 +7682,10 @@
         <v>3</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F11" s="10">
         <v>3</v>
@@ -7728,7 +7705,7 @@
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="B12" s="10">
         <v>10</v>
@@ -7737,10 +7714,10 @@
         <v>3</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F12" s="10">
         <v>3</v>
@@ -7760,7 +7737,7 @@
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="B13" s="10">
         <v>11</v>
@@ -7769,10 +7746,10 @@
         <v>2</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F13" s="10">
         <v>2</v>
@@ -7796,7 +7773,7 @@
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="B14" s="3">
         <v>12</v>
@@ -7805,10 +7782,10 @@
         <v>2</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F14" s="3">
         <v>2</v>
@@ -7833,7 +7810,7 @@
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="B15" s="3">
         <v>13</v>
@@ -7842,10 +7819,10 @@
         <v>1</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F15" s="3">
         <v>1</v>
@@ -7865,7 +7842,7 @@
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="B16" s="3">
         <v>14</v>
@@ -7874,10 +7851,10 @@
         <v>3</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F16" s="3">
         <v>3</v>
@@ -7905,7 +7882,7 @@
     </row>
     <row r="17" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="B17" s="3">
         <v>15</v>
@@ -7914,10 +7891,10 @@
         <v>3</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F17" s="3">
         <v>3</v>
@@ -7945,7 +7922,7 @@
     </row>
     <row r="18" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="B18" s="3">
         <v>16</v>
@@ -7954,10 +7931,10 @@
         <v>2</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F18" s="3">
         <v>2</v>
@@ -7985,7 +7962,7 @@
     </row>
     <row r="19" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="B19" s="3">
         <v>17</v>
@@ -7994,10 +7971,10 @@
         <v>2</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F19" s="3">
         <v>2</v>
@@ -8823,109 +8800,109 @@
     <mergeCell ref="G4:J4"/>
   </mergeCells>
   <conditionalFormatting sqref="A31:AE53 B21:AE30 A10:AE20">
-    <cfRule type="expression" dxfId="35" priority="28" stopIfTrue="1">
+    <cfRule type="expression" dxfId="32" priority="28" stopIfTrue="1">
       <formula>$E10="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="29" stopIfTrue="1">
+    <cfRule type="expression" dxfId="31" priority="29" stopIfTrue="1">
       <formula>$E10="Ongoing"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21 A30">
-    <cfRule type="expression" dxfId="33" priority="25" stopIfTrue="1">
+    <cfRule type="expression" dxfId="30" priority="25" stopIfTrue="1">
       <formula>$F21="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="29" priority="26" stopIfTrue="1">
       <formula>$F21="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="27" stopIfTrue="1">
+    <cfRule type="expression" dxfId="28" priority="27" stopIfTrue="1">
       <formula>$F21="Removed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A22">
-    <cfRule type="expression" dxfId="30" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="27" priority="22" stopIfTrue="1">
       <formula>$F22="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="29" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="26" priority="23" stopIfTrue="1">
       <formula>$F22="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="25" priority="24" stopIfTrue="1">
       <formula>$F22="Removed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A24">
-    <cfRule type="expression" dxfId="27" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="24" priority="19" stopIfTrue="1">
       <formula>$F24="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="23" priority="20" stopIfTrue="1">
       <formula>$F24="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="22" priority="21" stopIfTrue="1">
       <formula>$F24="Removed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A23">
-    <cfRule type="expression" dxfId="24" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="21" priority="16" stopIfTrue="1">
       <formula>$F23="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="20" priority="17" stopIfTrue="1">
       <formula>$F23="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="19" priority="18" stopIfTrue="1">
       <formula>$F23="Removed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A25">
-    <cfRule type="expression" dxfId="21" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="18" priority="13" stopIfTrue="1">
       <formula>$F25="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="17" priority="14" stopIfTrue="1">
       <formula>$F25="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="16" priority="15" stopIfTrue="1">
       <formula>$F25="Removed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A27">
-    <cfRule type="expression" dxfId="18" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="10" stopIfTrue="1">
       <formula>$F27="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="11" stopIfTrue="1">
       <formula>$F27="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="12" stopIfTrue="1">
       <formula>$F27="Removed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A29">
-    <cfRule type="expression" dxfId="15" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="7" stopIfTrue="1">
       <formula>$F29="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="8" stopIfTrue="1">
       <formula>$F29="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="9" stopIfTrue="1">
       <formula>$F29="Removed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A28">
-    <cfRule type="expression" dxfId="12" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="4" stopIfTrue="1">
       <formula>$F28="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="8" priority="5" stopIfTrue="1">
       <formula>$F28="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="7" priority="6" stopIfTrue="1">
       <formula>$F28="Removed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A26">
-    <cfRule type="expression" dxfId="9" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="1" stopIfTrue="1">
       <formula>$F26="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="2" stopIfTrue="1">
       <formula>$F26="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="3" stopIfTrue="1">
       <formula>$F26="Removed"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8948,7 +8925,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E13" sqref="E13"/>
+      <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -9025,7 +9002,7 @@
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" s="32" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="B4" s="33">
         <v>4</v>
@@ -9037,7 +9014,7 @@
         <v>2</v>
       </c>
       <c r="G4" s="48" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="H4" s="48"/>
       <c r="I4" s="48"/>
@@ -9066,7 +9043,7 @@
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" s="32" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B5" s="33">
         <v>2</v>
@@ -9183,17 +9160,17 @@
     </row>
     <row r="6" spans="1:31" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" s="37" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6" s="38">
         <f>IF(COUNTA(A10:A237)=0,1,COUNTA(A10:A237))</f>
         <v>6</v>
       </c>
       <c r="C6" s="37" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D6" s="37" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E6" s="38">
         <f ca="1">IF(COUNTIF(G5:AE5,"&gt;0")=0,1,COUNTIF(G5:AE5,"&gt;0"))</f>
@@ -9303,14 +9280,14 @@
     </row>
     <row r="7" spans="1:31" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" s="39" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B7" s="37"/>
       <c r="C7" s="37" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D7" s="37" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E7" s="38"/>
       <c r="F7" s="38"/>
@@ -9417,14 +9394,14 @@
     </row>
     <row r="8" spans="1:31" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" s="39" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B8" s="37"/>
       <c r="C8" s="37" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D8" s="37" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E8" s="38">
         <f ca="1">IF(DoneDays&gt;B5,B5,DoneDays)</f>
@@ -9510,13 +9487,13 @@
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" s="32" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B9" s="49" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C9" s="49" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D9" s="49" t="s">
         <v>1</v>
@@ -9629,7 +9606,7 @@
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="B10" s="15">
         <v>18</v>
@@ -9638,10 +9615,10 @@
         <v>2</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F10" s="10">
         <v>2</v>
@@ -9657,7 +9634,7 @@
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="B11" s="15">
         <v>19</v>
@@ -9666,10 +9643,10 @@
         <v>3</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F11" s="10">
         <v>3</v>
@@ -9687,7 +9664,7 @@
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="B12" s="15">
         <v>20</v>
@@ -9696,10 +9673,10 @@
         <v>3</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F12" s="10">
         <v>3</v>
@@ -9717,7 +9694,7 @@
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="B13" s="15">
         <v>21</v>
@@ -9726,10 +9703,10 @@
         <v>3</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E13" s="15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F13" s="10">
         <v>3</v>
@@ -9757,7 +9734,7 @@
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B14" s="15">
         <v>22</v>
@@ -9766,10 +9743,10 @@
         <v>5</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E14" s="15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F14" s="3">
         <v>5</v>
@@ -9798,7 +9775,7 @@
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B15" s="15">
         <v>23</v>
@@ -9807,10 +9784,10 @@
         <v>5</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E15" s="15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F15" s="3">
         <v>5</v>
@@ -10811,18 +10788,18 @@
     <mergeCell ref="G4:J4"/>
   </mergeCells>
   <conditionalFormatting sqref="A10:B53 D10:AE53">
-    <cfRule type="expression" dxfId="6" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="3" priority="3" stopIfTrue="1">
       <formula>$E10="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="2" priority="4" stopIfTrue="1">
       <formula>$E10="Ongoing"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10:C53">
-    <cfRule type="expression" dxfId="4" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="1" priority="1" stopIfTrue="1">
       <formula>$E10="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="0" priority="2" stopIfTrue="1">
       <formula>$E10="Ongoing"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>